<commit_message>
tests Zhao 30 and 50 nt
</commit_message>
<xml_diff>
--- a/Article/AdditionalData/2010_ExpressionAnalysisCompare.xlsx
+++ b/Article/AdditionalData/2010_ExpressionAnalysisCompare.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
   <si>
     <t xml:space="preserve">Author:</t>
   </si>
@@ -234,7 +234,13 @@
     <t xml:space="preserve">Meng 40 end</t>
   </si>
   <si>
+    <t xml:space="preserve">Zhao 30 start</t>
+  </si>
+  <si>
     <t xml:space="preserve">Zhao 40 start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zhao 50 start</t>
   </si>
   <si>
     <t xml:space="preserve">Neves et al (unpubl)</t>
@@ -468,11 +474,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,51 +517,51 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -575,811 +581,919 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.06</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>0.43</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="O2" s="1" t="n">
+      <c r="O2" s="2" t="n">
         <f aca="false">N2/M2</f>
         <v>0.465116279069768</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>0.58</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>0.62</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>0.44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>0.61</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>0.38</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>0.18</v>
       </c>
-      <c r="O3" s="1" t="n">
+      <c r="O3" s="2" t="n">
         <f aca="false">N3/M3</f>
         <v>0.473684210526316</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>0.81</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>0.42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>709</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>0.39</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O4" s="1" t="n">
+      <c r="O4" s="2" t="n">
         <f aca="false">N4/M4</f>
         <v>0.41025641025641</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <v>0.84</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <v>0.12</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="S4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>0.22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>3188</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <v>355</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>285</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>0.09</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.61</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="N5" s="1" t="n">
         <v>0.03</v>
       </c>
-      <c r="O5" s="1" t="n">
+      <c r="O5" s="2" t="n">
         <f aca="false">N5/M5</f>
         <v>0.0491803278688525</v>
       </c>
-      <c r="P5" s="0" t="n">
+      <c r="P5" s="1" t="n">
         <v>0.63</v>
       </c>
-      <c r="Q5" s="0" t="n">
+      <c r="Q5" s="1" t="n">
         <v>0.65</v>
       </c>
-      <c r="R5" s="0" t="n">
+      <c r="R5" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="S5" s="0" t="s">
+      <c r="S5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="T5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="U5" s="0" t="n">
+      <c r="U5" s="1" t="n">
         <v>0.24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="I6" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>397</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="1" t="n">
         <v>0.69</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
         <v>0.27</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="N6" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O6" s="1" t="n">
+      <c r="O6" s="2" t="n">
         <f aca="false">N6/M6</f>
         <v>0.592592592592593</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="P6" s="1" t="n">
         <v>0.99</v>
       </c>
-      <c r="Q6" s="0" t="n">
+      <c r="Q6" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="R6" s="0" t="n">
+      <c r="R6" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="S6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="T6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U6" s="0" t="n">
+      <c r="U6" s="1" t="n">
         <v>0.11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="I7" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>397</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="L7" s="1" t="n">
         <v>0.69</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="M7" s="1" t="n">
         <v>0.29</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="N7" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O7" s="1" t="n">
+      <c r="O7" s="2" t="n">
         <f aca="false">N7/M7</f>
         <v>0.551724137931035</v>
       </c>
-      <c r="P7" s="0" t="n">
+      <c r="P7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Q7" s="0" t="n">
+      <c r="Q7" s="1" t="n">
         <v>0.21</v>
       </c>
-      <c r="R7" s="0" t="n">
+      <c r="R7" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="S7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="T7" s="0" t="s">
+      <c r="T7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="U7" s="0" t="n">
+      <c r="U7" s="1" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="I8" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="J8" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="1" t="n">
         <v>0.35</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="M8" s="1" t="n">
         <v>0.56</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="N8" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="O8" s="1" t="n">
+      <c r="O8" s="2" t="n">
         <f aca="false">N8/M8</f>
         <v>0.142857142857143</v>
       </c>
-      <c r="P8" s="0" t="n">
+      <c r="P8" s="1" t="n">
         <v>0.84</v>
       </c>
-      <c r="Q8" s="0" t="n">
+      <c r="Q8" s="1" t="n">
         <v>0.59</v>
       </c>
-      <c r="R8" s="0" t="n">
+      <c r="R8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="S8" s="0" t="s">
+      <c r="S8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="T8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="U8" s="0" t="n">
+      <c r="U8" s="1" t="n">
         <v>0.37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="I9" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="J9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="K9" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="L9" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="M9" s="1" t="n">
         <v>0.22</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="N9" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="O9" s="1" t="n">
+      <c r="O9" s="2" t="n">
         <f aca="false">N9/M9</f>
         <v>0.681818181818182</v>
       </c>
-      <c r="P9" s="0" t="n">
+      <c r="P9" s="1" t="n">
         <v>0.69</v>
       </c>
-      <c r="Q9" s="0" t="n">
+      <c r="Q9" s="1" t="n">
         <v>0.56</v>
       </c>
-      <c r="U9" s="0" t="n">
+      <c r="U9" s="1" t="n">
         <v>0.31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="I10" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="J10" s="0" t="n">
+      <c r="J10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="K10" s="0" t="n">
+      <c r="K10" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="L10" s="0" t="n">
+      <c r="L10" s="1" t="n">
         <v>0.21</v>
       </c>
-      <c r="M10" s="0" t="n">
+      <c r="M10" s="1" t="n">
         <v>0.36</v>
       </c>
-      <c r="N10" s="0" t="n">
+      <c r="N10" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="O10" s="1" t="n">
+      <c r="O10" s="2" t="n">
         <f aca="false">N10/M10</f>
         <v>0.388888888888889</v>
       </c>
-      <c r="P10" s="0" t="n">
+      <c r="P10" s="1" t="n">
         <v>0.71</v>
       </c>
-      <c r="Q10" s="0" t="n">
+      <c r="Q10" s="1" t="n">
         <v>0.47</v>
       </c>
-      <c r="U10" s="0" t="n">
+      <c r="U10" s="1" t="n">
         <v>0.42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>416</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <f aca="false">N11/M11</f>
+        <v>0.129032258064516</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="U11" s="1" t="n">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I12" s="1" t="n">
         <v>806</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J12" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K12" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L12" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M12" s="1" t="n">
         <v>0.59</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N12" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="O11" s="1" t="n">
-        <f aca="false">N11/M11</f>
+      <c r="O12" s="2" t="n">
+        <f aca="false">N12/M12</f>
         <v>0.0847457627118644</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P12" s="1" t="n">
         <v>0.61</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q12" s="1" t="n">
         <v>0.55</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="U12" s="1" t="n">
         <v>0.43</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="0" t="s">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G13" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1818</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <f aca="false">N13/M13</f>
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="U13" s="1" t="n">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="I14" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J14" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="K14" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L14" s="1" t="n">
         <v>0.42</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M14" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N14" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O12" s="1" t="n">
-        <f aca="false">N12/M12</f>
+      <c r="O14" s="2" t="n">
+        <f aca="false">N14/M14</f>
         <v>0.266666666666667</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="P14" s="1" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q14" s="1" t="n">
         <v>0.64</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U14" s="1" t="n">
         <v>0.63</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="0" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J15" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="K13" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="L13" s="0" t="n">
+      <c r="L15" s="1" t="n">
         <v>0.42</v>
       </c>
-      <c r="M13" s="0" t="n">
+      <c r="M15" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="N13" s="0" t="n">
+      <c r="N15" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="O13" s="1" t="n">
-        <f aca="false">N13/M13</f>
+      <c r="O15" s="2" t="n">
+        <f aca="false">N15/M15</f>
         <v>0.233333333333333</v>
       </c>
-      <c r="P13" s="0" t="n">
+      <c r="P15" s="1" t="n">
         <v>0.87</v>
       </c>
-      <c r="Q13" s="0" t="n">
+      <c r="Q15" s="1" t="n">
         <v>0.58</v>
       </c>
-      <c r="U13" s="0" t="n">
+      <c r="U15" s="1" t="n">
         <v>0.34</v>
       </c>
     </row>
@@ -1405,51 +1519,51 @@
       <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" s="1" t="n">
+      <c r="A2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>6.69359239669702</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="1" t="n">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>6.87560340600088</v>
       </c>
       <c r="H3" s="3"/>
@@ -1458,16 +1572,16 @@
       <c r="Q3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>6.61582549966695</v>
       </c>
       <c r="H4" s="3"/>
@@ -1476,471 +1590,471 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="1" t="n">
+      <c r="A5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>6.82761650850118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="1" t="n">
+      <c r="A6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>6.66674964520377</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="1" t="n">
+      <c r="A7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>6.3501856367314</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="1" t="n">
+      <c r="A8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>6.35723262874483</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="1" t="n">
+      <c r="A9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>6.143212917343</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="1" t="n">
+      <c r="A10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="2" t="n">
         <v>9.3422993</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>6.0529411810276</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>88</v>
+      <c r="A11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D11" s="1" t="n">
         <v>4.8368103979843</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="C12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>7.80912530132803</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>88</v>
+      <c r="A13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D13" s="1" t="n">
         <v>7.45718354223775</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>88</v>
+      <c r="A14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>6.92315722921499</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>88</v>
+      <c r="A15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D15" s="1" t="n">
         <v>7.12612421266836</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>88</v>
+      <c r="A16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D16" s="1" t="n">
         <v>7.01509154869803</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>88</v>
+      <c r="A17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D17" s="1" t="n">
         <v>7.9257459912934</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>88</v>
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D18" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D18" s="1" t="n">
         <v>7.58034571657039</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>88</v>
+      <c r="A19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1" t="n">
         <v>7.15629266929003</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>100</v>
+      <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1" t="n">
         <v>6.77196534936234</v>
       </c>
-      <c r="E20" s="0" t="s">
-        <v>101</v>
+      <c r="E20" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>100</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="n">
         <v>6.88940549233399</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>100</v>
+      <c r="A22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <v>6.58194439497502</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>100</v>
+      <c r="A23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="n">
         <v>9.75216192831353</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>100</v>
+      <c r="A24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D24" s="1" t="n">
         <v>11.3590632558959</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>100</v>
+      <c r="A25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D25" s="1" t="n">
         <v>10.9221707907588</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>100</v>
+      <c r="A26" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D26" s="1" t="n">
         <v>13.5869345709037</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>100</v>
+      <c r="A27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D27" s="1" t="n">
         <v>12.603648513987</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>100</v>
+      <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="D28" s="1" t="n">
         <v>8.81433172368548</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="1" t="s">
         <v>112</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>20.0543958948375</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="C30" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="D30" s="6" t="n">
         <v>21.0286917060505</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>112</v>
+      <c r="A31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D31" s="6" t="n">
         <v>19.830674037943</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>112</v>
+      <c r="A32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D32" s="6" t="n">
         <v>18.2253079472565</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>112</v>
+      <c r="A33" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D33" s="6" t="n">
         <v>17.0749779487674</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>112</v>
+      <c r="A34" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D34" s="6" t="n">
         <v>18.3108979096254</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>112</v>
+      <c r="A35" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D35" s="6" t="n">
         <v>17.4050552492193</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>112</v>
+      <c r="A36" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D36" s="6" t="n">
         <v>16.4378937441482</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>112</v>
+      <c r="A37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="D37" s="6" t="n">
         <v>15.8994589314662</v>

</xml_diff>

<commit_message>
add further cross test
</commit_message>
<xml_diff>
--- a/Article/AdditionalData/2010_ExpressionAnalysisCompare.xlsx
+++ b/Article/AdditionalData/2010_ExpressionAnalysisCompare.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="125">
   <si>
     <t xml:space="preserve">Author:</t>
   </si>
@@ -36,13 +36,16 @@
     <t xml:space="preserve">ulf.liebal@rwth-aachen.de</t>
   </si>
   <si>
-    <t xml:space="preserve">Relation:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This file belongs to the article ’Insight to gene expression from promoter libraries with the machine learning workflow Exp2Ipynb’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOI:</t>
+    <t xml:space="preserve">Parent Article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insight to gene expression from promoter libraries with the machine learning workflow Exp2Ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Article DOI:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.3389/fbinf.2021.747428</t>
   </si>
   <si>
     <t xml:space="preserve">Content:</t>
@@ -478,12 +481,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -517,11 +520,14 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.62"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -551,18 +557,21 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -583,11 +592,11 @@
   </sheetPr>
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.14"/>
@@ -600,84 +609,84 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="n">
         <v>0.2</v>
@@ -703,7 +712,7 @@
       <c r="N2" s="1" t="n">
         <v>0.2</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="3" t="n">
         <f aca="false">N2/M2</f>
         <v>0.465116279069768</v>
       </c>
@@ -717,10 +726,10 @@
         <v>2</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U2" s="1" t="n">
         <v>0.44</v>
@@ -728,22 +737,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G3" s="1" t="n">
         <v>1</v>
@@ -769,7 +778,7 @@
       <c r="N3" s="1" t="n">
         <v>0.18</v>
       </c>
-      <c r="O3" s="2" t="n">
+      <c r="O3" s="3" t="n">
         <f aca="false">N3/M3</f>
         <v>0.473684210526316</v>
       </c>
@@ -783,10 +792,10 @@
         <v>10</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U3" s="1" t="n">
         <v>0.42</v>
@@ -794,22 +803,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="n">
         <v>0.2</v>
@@ -835,7 +844,7 @@
       <c r="N4" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O4" s="2" t="n">
+      <c r="O4" s="3" t="n">
         <f aca="false">N4/M4</f>
         <v>0.41025641025641</v>
       </c>
@@ -849,10 +858,10 @@
         <v>5</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U4" s="1" t="n">
         <v>0.22</v>
@@ -860,22 +869,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="n">
         <v>0.2</v>
@@ -901,7 +910,7 @@
       <c r="N5" s="1" t="n">
         <v>0.03</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="O5" s="3" t="n">
         <f aca="false">N5/M5</f>
         <v>0.0491803278688525</v>
       </c>
@@ -915,10 +924,10 @@
         <v>6</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U5" s="1" t="n">
         <v>0.24</v>
@@ -926,22 +935,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G6" s="1" t="n">
         <v>1</v>
@@ -967,7 +976,7 @@
       <c r="N6" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="O6" s="3" t="n">
         <f aca="false">N6/M6</f>
         <v>0.592592592592593</v>
       </c>
@@ -981,10 +990,10 @@
         <v>20</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U6" s="1" t="n">
         <v>0.11</v>
@@ -992,22 +1001,22 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>1</v>
@@ -1033,7 +1042,7 @@
       <c r="N7" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="O7" s="3" t="n">
         <f aca="false">N7/M7</f>
         <v>0.551724137931035</v>
       </c>
@@ -1047,10 +1056,10 @@
         <v>128</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U7" s="1" t="n">
         <v>0.08</v>
@@ -1058,22 +1067,22 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G8" s="1" t="n">
         <v>1</v>
@@ -1099,7 +1108,7 @@
       <c r="N8" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="O8" s="2" t="n">
+      <c r="O8" s="3" t="n">
         <f aca="false">N8/M8</f>
         <v>0.142857142857143</v>
       </c>
@@ -1113,10 +1122,10 @@
         <v>7</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U8" s="1" t="n">
         <v>0.37</v>
@@ -1124,19 +1133,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="n">
         <v>0.2</v>
@@ -1159,7 +1168,7 @@
       <c r="N9" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="O9" s="3" t="n">
         <f aca="false">N9/M9</f>
         <v>0.681818181818182</v>
       </c>
@@ -1175,19 +1184,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>0.2</v>
@@ -1213,7 +1222,7 @@
       <c r="N10" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="O10" s="2" t="n">
+      <c r="O10" s="3" t="n">
         <f aca="false">N10/M10</f>
         <v>0.388888888888889</v>
       </c>
@@ -1229,19 +1238,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="n">
         <v>0.2</v>
@@ -1267,7 +1276,7 @@
       <c r="N11" s="1" t="n">
         <v>0.08</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="O11" s="3" t="n">
         <f aca="false">N11/M11</f>
         <v>0.129032258064516</v>
       </c>
@@ -1283,19 +1292,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="n">
         <v>0.2</v>
@@ -1321,7 +1330,7 @@
       <c r="N12" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="O12" s="2" t="n">
+      <c r="O12" s="3" t="n">
         <f aca="false">N12/M12</f>
         <v>0.0847457627118644</v>
       </c>
@@ -1337,19 +1346,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>0.2</v>
@@ -1375,7 +1384,7 @@
       <c r="N13" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="O13" s="3" t="n">
         <f aca="false">N13/M13</f>
         <v>0.0833333333333333</v>
       </c>
@@ -1391,19 +1400,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G14" s="1" t="n">
         <v>1</v>
@@ -1429,7 +1438,7 @@
       <c r="N14" s="1" t="n">
         <v>0.16</v>
       </c>
-      <c r="O14" s="2" t="n">
+      <c r="O14" s="3" t="n">
         <f aca="false">N14/M14</f>
         <v>0.266666666666667</v>
       </c>
@@ -1445,19 +1454,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="1" t="n">
         <v>1</v>
@@ -1483,7 +1492,7 @@
       <c r="N15" s="1" t="n">
         <v>0.14</v>
       </c>
-      <c r="O15" s="2" t="n">
+      <c r="O15" s="3" t="n">
         <f aca="false">N15/M15</f>
         <v>0.233333333333333</v>
       </c>
@@ -1515,38 +1524,38 @@
   </sheetPr>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.87"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D2" s="1" t="n">
@@ -1555,48 +1564,48 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>6.87560340600088</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C4" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>6.61582549966695</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="O4" s="3"/>
+      <c r="H4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C5" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D5" s="1" t="n">
@@ -1605,12 +1614,12 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C6" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D6" s="1" t="n">
@@ -1619,12 +1628,12 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C7" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D7" s="1" t="n">
@@ -1633,12 +1642,12 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D8" s="1" t="n">
@@ -1647,12 +1656,12 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C9" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D9" s="1" t="n">
@@ -1661,12 +1670,12 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="2" t="n">
+        <v>81</v>
+      </c>
+      <c r="C10" s="3" t="n">
         <v>9.3422993</v>
       </c>
       <c r="D10" s="1" t="n">
@@ -1675,30 +1684,30 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>4.8368103979843</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>7.80912530132803</v>
@@ -1706,13 +1715,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" s="1" t="n">
         <v>7.45718354223775</v>
@@ -1720,13 +1729,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D14" s="1" t="n">
         <v>6.92315722921499</v>
@@ -1734,13 +1743,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D15" s="1" t="n">
         <v>7.12612421266836</v>
@@ -1748,13 +1757,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D16" s="1" t="n">
         <v>7.01509154869803</v>
@@ -1762,13 +1771,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D17" s="1" t="n">
         <v>7.9257459912934</v>
@@ -1776,13 +1785,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D18" s="1" t="n">
         <v>7.58034571657039</v>
@@ -1790,13 +1799,13 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D19" s="1" t="n">
         <v>7.15629266929003</v>
@@ -1804,30 +1813,30 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1" t="n">
         <v>6.77196534936234</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D21" s="1" t="n">
         <v>6.88940549233399</v>
@@ -1835,13 +1844,13 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="n">
         <v>6.58194439497502</v>
@@ -1849,13 +1858,13 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D23" s="1" t="n">
         <v>9.75216192831353</v>
@@ -1863,13 +1872,13 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D24" s="1" t="n">
         <v>11.3590632558959</v>
@@ -1877,13 +1886,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="1" t="n">
         <v>10.9221707907588</v>
@@ -1891,13 +1900,13 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D26" s="1" t="n">
         <v>13.5869345709037</v>
@@ -1905,13 +1914,13 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>12.603648513987</v>
@@ -1919,13 +1928,13 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" s="1" t="n">
         <v>8.81433172368548</v>
@@ -1933,30 +1942,30 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>20.0543958948375</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D30" s="6" t="n">
         <v>21.0286917060505</v>
@@ -1964,13 +1973,13 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D31" s="6" t="n">
         <v>19.830674037943</v>
@@ -1978,13 +1987,13 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D32" s="6" t="n">
         <v>18.2253079472565</v>
@@ -1992,13 +2001,13 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D33" s="6" t="n">
         <v>17.0749779487674</v>
@@ -2006,13 +2015,13 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D34" s="6" t="n">
         <v>18.3108979096254</v>
@@ -2020,13 +2029,13 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D35" s="6" t="n">
         <v>17.4050552492193</v>
@@ -2034,13 +2043,13 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D36" s="6" t="n">
         <v>16.4378937441482</v>
@@ -2048,13 +2057,13 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="2" t="s">
         <v>114</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="D37" s="6" t="n">
         <v>15.8994589314662</v>

</xml_diff>